<commit_message>
Mejora rendimiento y visualización
</commit_message>
<xml_diff>
--- a/Financiero.xlsx
+++ b/Financiero.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Proveedores" sheetId="1" state="visible" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00;\-&quot;$&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="167" formatCode="D/M/YYYY"/>
+    <numFmt numFmtId="167" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="168" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="3">
@@ -113,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -139,8 +139,9 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -280,8 +281,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Resumen" displayName="Resumen" ref="A1:D4" headerRowCount="1" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:D4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Resumen" displayName="Resumen" ref="B1:E7" headerRowCount="1" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="B1:E7"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Proveedor"/>
     <tableColumn id="2" name="Total Facturas" dataDxfId="1"/>
@@ -613,7 +614,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F148"/>
+  <dimension ref="A1:F153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:F1"/>
@@ -634,7 +635,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fecha </t>
+          <t>Fecha</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
@@ -649,7 +650,7 @@
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>Observación</t>
+          <t>Obs</t>
         </is>
       </c>
       <c r="F1" s="2" t="inlineStr">
@@ -662,7 +663,7 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="n">
+      <c r="B2" s="14" t="n">
         <v>45816</v>
       </c>
       <c r="C2" t="inlineStr">
@@ -680,7 +681,7 @@
           <t>Saldo</t>
         </is>
       </c>
-      <c r="F2" s="12" t="n">
+      <c r="F2" t="n">
         <v>52433000</v>
       </c>
     </row>
@@ -688,7 +689,7 @@
       <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="n">
+      <c r="B3" s="14" t="n">
         <v>45816</v>
       </c>
       <c r="C3" t="inlineStr">
@@ -706,7 +707,7 @@
           <t>Compra</t>
         </is>
       </c>
-      <c r="F3" s="12" t="n">
+      <c r="F3" t="n">
         <v>26354000</v>
       </c>
     </row>
@@ -714,7 +715,7 @@
       <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="14" t="n">
         <v>45818</v>
       </c>
       <c r="C4" t="inlineStr">
@@ -732,7 +733,7 @@
           <t>Compra</t>
         </is>
       </c>
-      <c r="F4" s="12" t="n">
+      <c r="F4" t="n">
         <v>19129000</v>
       </c>
     </row>
@@ -740,7 +741,7 @@
       <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="n">
+      <c r="B5" s="14" t="n">
         <v>45820</v>
       </c>
       <c r="C5" t="inlineStr">
@@ -758,7 +759,7 @@
           <t>Compra</t>
         </is>
       </c>
-      <c r="F5" s="12" t="n">
+      <c r="F5" t="n">
         <v>54840000</v>
       </c>
     </row>
@@ -766,7 +767,7 @@
       <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="n">
+      <c r="B6" s="14" t="n">
         <v>45828</v>
       </c>
       <c r="C6" t="inlineStr">
@@ -784,7 +785,7 @@
           <t>Compra</t>
         </is>
       </c>
-      <c r="F6" s="12" t="n">
+      <c r="F6" t="n">
         <v>63918000</v>
       </c>
     </row>
@@ -792,7 +793,7 @@
       <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="n">
+      <c r="B7" s="14" t="n">
         <v>45843</v>
       </c>
       <c r="C7" t="inlineStr">
@@ -810,7 +811,7 @@
           <t>Compra</t>
         </is>
       </c>
-      <c r="F7" s="12" t="n">
+      <c r="F7" t="n">
         <v>136060000</v>
       </c>
     </row>
@@ -818,7 +819,7 @@
       <c r="A8" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="n">
+      <c r="B8" s="14" t="n">
         <v>45848</v>
       </c>
       <c r="C8" t="inlineStr">
@@ -836,7 +837,7 @@
           <t>Compra</t>
         </is>
       </c>
-      <c r="F8" s="12" t="n">
+      <c r="F8" t="n">
         <v>98794250</v>
       </c>
     </row>
@@ -844,7 +845,7 @@
       <c r="A9" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="n">
+      <c r="B9" s="14" t="n">
         <v>45849</v>
       </c>
       <c r="C9" t="inlineStr">
@@ -862,7 +863,7 @@
           <t>Compra</t>
         </is>
       </c>
-      <c r="F9" s="12" t="n">
+      <c r="F9" t="n">
         <v>44541000</v>
       </c>
     </row>
@@ -870,7 +871,7 @@
       <c r="A10" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="n">
+      <c r="B10" s="14" t="n">
         <v>45863</v>
       </c>
       <c r="C10" t="inlineStr">
@@ -888,7 +889,7 @@
           <t>Compra</t>
         </is>
       </c>
-      <c r="F10" s="12" t="n">
+      <c r="F10" t="n">
         <v>126125800</v>
       </c>
     </row>
@@ -896,7 +897,7 @@
       <c r="A11" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="n">
+      <c r="B11" s="14" t="n">
         <v>45807</v>
       </c>
       <c r="C11" t="inlineStr">
@@ -914,7 +915,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F11" s="12" t="n">
+      <c r="F11" t="n">
         <v>13828960</v>
       </c>
     </row>
@@ -922,7 +923,7 @@
       <c r="A12" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="11" t="n">
+      <c r="B12" s="14" t="n">
         <v>45807</v>
       </c>
       <c r="C12" t="inlineStr">
@@ -940,7 +941,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F12" s="12" t="n">
+      <c r="F12" t="n">
         <v>26554608</v>
       </c>
     </row>
@@ -948,7 +949,7 @@
       <c r="A13" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="n">
+      <c r="B13" s="14" t="n">
         <v>45722</v>
       </c>
       <c r="C13" t="inlineStr">
@@ -966,7 +967,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F13" s="12" t="n">
+      <c r="F13" t="n">
         <v>12050000</v>
       </c>
     </row>
@@ -974,7 +975,7 @@
       <c r="A14" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="n">
+      <c r="B14" s="14" t="n">
         <v>45819</v>
       </c>
       <c r="C14" t="inlineStr">
@@ -992,7 +993,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F14" s="12" t="n">
+      <c r="F14" t="n">
         <v>45000000</v>
       </c>
     </row>
@@ -1000,7 +1001,7 @@
       <c r="A15" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="n">
+      <c r="B15" s="14" t="n">
         <v>45820</v>
       </c>
       <c r="C15" t="inlineStr">
@@ -1018,7 +1019,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F15" s="12" t="n">
+      <c r="F15" t="n">
         <v>9000000</v>
       </c>
     </row>
@@ -1026,7 +1027,7 @@
       <c r="A16" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="n">
+      <c r="B16" s="14" t="n">
         <v>45822</v>
       </c>
       <c r="C16" t="inlineStr">
@@ -1044,7 +1045,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F16" s="12" t="n">
+      <c r="F16" t="n">
         <v>5994800</v>
       </c>
     </row>
@@ -1052,7 +1053,7 @@
       <c r="A17" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="n">
+      <c r="B17" s="14" t="n">
         <v>45822</v>
       </c>
       <c r="C17" t="inlineStr">
@@ -1070,7 +1071,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F17" s="12" t="n">
+      <c r="F17" t="n">
         <v>5341300</v>
       </c>
     </row>
@@ -1078,7 +1079,7 @@
       <c r="A18" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="n">
+      <c r="B18" s="14" t="n">
         <v>45822</v>
       </c>
       <c r="C18" t="inlineStr">
@@ -1096,7 +1097,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F18" s="12" t="n">
+      <c r="F18" t="n">
         <v>18976000</v>
       </c>
     </row>
@@ -1104,7 +1105,7 @@
       <c r="A19" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="4" t="n">
+      <c r="B19" s="14" t="n">
         <v>45829</v>
       </c>
       <c r="C19" t="inlineStr">
@@ -1122,7 +1123,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F19" s="12" t="n">
+      <c r="F19" t="n">
         <v>10000000</v>
       </c>
     </row>
@@ -1130,7 +1131,7 @@
       <c r="A20" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="n">
+      <c r="B20" s="14" t="n">
         <v>45833</v>
       </c>
       <c r="C20" t="inlineStr">
@@ -1148,7 +1149,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F20" s="12" t="n">
+      <c r="F20" t="n">
         <v>10000000</v>
       </c>
     </row>
@@ -1156,7 +1157,7 @@
       <c r="A21" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="n">
+      <c r="B21" s="14" t="n">
         <v>45836</v>
       </c>
       <c r="C21" t="inlineStr">
@@ -1174,7 +1175,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F21" s="12" t="n">
+      <c r="F21" t="n">
         <v>10000000</v>
       </c>
     </row>
@@ -1182,7 +1183,7 @@
       <c r="A22" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="n">
+      <c r="B22" s="14" t="n">
         <v>45839</v>
       </c>
       <c r="C22" t="inlineStr">
@@ -1200,7 +1201,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F22" s="12" t="n">
+      <c r="F22" t="n">
         <v>20000000</v>
       </c>
     </row>
@@ -1208,7 +1209,7 @@
       <c r="A23" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="n">
+      <c r="B23" s="14" t="n">
         <v>45839</v>
       </c>
       <c r="C23" t="inlineStr">
@@ -1226,7 +1227,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F23" s="12" t="n">
+      <c r="F23" t="n">
         <v>10000000</v>
       </c>
     </row>
@@ -1234,7 +1235,7 @@
       <c r="A24" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="4" t="n">
+      <c r="B24" s="14" t="n">
         <v>45839</v>
       </c>
       <c r="C24" t="inlineStr">
@@ -1252,7 +1253,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F24" s="12" t="n">
+      <c r="F24" t="n">
         <v>4000000</v>
       </c>
     </row>
@@ -1260,7 +1261,7 @@
       <c r="A25" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="4" t="n">
+      <c r="B25" s="14" t="n">
         <v>45839</v>
       </c>
       <c r="C25" t="inlineStr">
@@ -1278,7 +1279,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F25" s="12" t="n">
+      <c r="F25" t="n">
         <v>18500000</v>
       </c>
     </row>
@@ -1286,7 +1287,7 @@
       <c r="A26" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="4" t="n">
+      <c r="B26" s="14" t="n">
         <v>45840</v>
       </c>
       <c r="C26" t="inlineStr">
@@ -1304,7 +1305,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F26" s="12" t="n">
+      <c r="F26" t="n">
         <v>10000000</v>
       </c>
     </row>
@@ -1312,7 +1313,7 @@
       <c r="A27" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="4" t="n">
+      <c r="B27" s="14" t="n">
         <v>45840</v>
       </c>
       <c r="C27" t="inlineStr">
@@ -1330,7 +1331,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F27" s="12" t="n">
+      <c r="F27" t="n">
         <v>10089200</v>
       </c>
     </row>
@@ -1338,7 +1339,7 @@
       <c r="A28" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="4" t="n">
+      <c r="B28" s="14" t="n">
         <v>45840</v>
       </c>
       <c r="C28" t="inlineStr">
@@ -1356,7 +1357,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F28" s="12" t="n">
+      <c r="F28" t="n">
         <v>16994000</v>
       </c>
     </row>
@@ -1364,7 +1365,7 @@
       <c r="A29" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="4" t="n">
+      <c r="B29" s="14" t="n">
         <v>45841</v>
       </c>
       <c r="C29" t="inlineStr">
@@ -1382,7 +1383,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F29" s="12" t="n">
+      <c r="F29" t="n">
         <v>5500000</v>
       </c>
     </row>
@@ -1390,7 +1391,7 @@
       <c r="A30" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="4" t="n">
+      <c r="B30" s="14" t="n">
         <v>45841</v>
       </c>
       <c r="C30" t="inlineStr">
@@ -1408,7 +1409,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F30" s="12" t="n">
+      <c r="F30" t="n">
         <v>6000000</v>
       </c>
     </row>
@@ -1416,7 +1417,7 @@
       <c r="A31" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="4" t="n">
+      <c r="B31" s="14" t="n">
         <v>45841</v>
       </c>
       <c r="C31" t="inlineStr">
@@ -1434,7 +1435,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F31" s="12" t="n">
+      <c r="F31" t="n">
         <v>4000000</v>
       </c>
     </row>
@@ -1442,7 +1443,7 @@
       <c r="A32" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="4" t="n">
+      <c r="B32" s="14" t="n">
         <v>45841</v>
       </c>
       <c r="C32" t="inlineStr">
@@ -1460,7 +1461,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F32" s="12" t="n">
+      <c r="F32" t="n">
         <v>14064000</v>
       </c>
     </row>
@@ -1468,7 +1469,7 @@
       <c r="A33" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="4" t="n">
+      <c r="B33" s="14" t="n">
         <v>45841</v>
       </c>
       <c r="C33" t="inlineStr">
@@ -1486,7 +1487,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F33" s="12" t="n">
+      <c r="F33" t="n">
         <v>19450000</v>
       </c>
     </row>
@@ -1494,7 +1495,7 @@
       <c r="A34" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="4" t="n">
+      <c r="B34" s="14" t="n">
         <v>45842</v>
       </c>
       <c r="C34" t="inlineStr">
@@ -1512,7 +1513,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F34" s="12" t="n">
+      <c r="F34" t="n">
         <v>22000000</v>
       </c>
     </row>
@@ -1520,7 +1521,7 @@
       <c r="A35" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="4" t="n">
+      <c r="B35" s="14" t="n">
         <v>45847</v>
       </c>
       <c r="C35" t="inlineStr">
@@ -1538,7 +1539,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F35" s="12" t="n">
+      <c r="F35" t="n">
         <v>17000000</v>
       </c>
     </row>
@@ -1546,7 +1547,7 @@
       <c r="A36" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="4" t="n">
+      <c r="B36" s="14" t="n">
         <v>45847</v>
       </c>
       <c r="C36" t="inlineStr">
@@ -1564,7 +1565,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F36" s="12" t="n">
+      <c r="F36" t="n">
         <v>3000000</v>
       </c>
     </row>
@@ -1572,7 +1573,7 @@
       <c r="A37" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="4" t="n">
+      <c r="B37" s="14" t="n">
         <v>45847</v>
       </c>
       <c r="C37" t="inlineStr">
@@ -1590,7 +1591,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F37" s="12" t="n">
+      <c r="F37" t="n">
         <v>3000000</v>
       </c>
     </row>
@@ -1598,7 +1599,7 @@
       <c r="A38" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="4" t="n">
+      <c r="B38" s="14" t="n">
         <v>45847</v>
       </c>
       <c r="C38" t="inlineStr">
@@ -1616,7 +1617,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F38" s="12" t="n">
+      <c r="F38" t="n">
         <v>1480000</v>
       </c>
     </row>
@@ -1624,7 +1625,7 @@
       <c r="A39" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="4" t="n">
+      <c r="B39" s="14" t="n">
         <v>45847</v>
       </c>
       <c r="C39" t="inlineStr">
@@ -1642,7 +1643,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F39" s="12" t="n">
+      <c r="F39" t="n">
         <v>2133000</v>
       </c>
     </row>
@@ -1650,7 +1651,7 @@
       <c r="A40" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="4" t="n">
+      <c r="B40" s="14" t="n">
         <v>45847</v>
       </c>
       <c r="C40" t="inlineStr">
@@ -1668,7 +1669,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F40" s="12" t="n">
+      <c r="F40" t="n">
         <v>3000000</v>
       </c>
     </row>
@@ -1676,7 +1677,7 @@
       <c r="A41" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="4" t="n">
+      <c r="B41" s="14" t="n">
         <v>45847</v>
       </c>
       <c r="C41" t="inlineStr">
@@ -1694,7 +1695,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F41" s="12" t="n">
+      <c r="F41" t="n">
         <v>80000</v>
       </c>
     </row>
@@ -1702,7 +1703,7 @@
       <c r="A42" t="n">
         <v>41</v>
       </c>
-      <c r="B42" s="4" t="n">
+      <c r="B42" s="14" t="n">
         <v>45847</v>
       </c>
       <c r="C42" t="inlineStr">
@@ -1720,7 +1721,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F42" s="12" t="n">
+      <c r="F42" t="n">
         <v>64087000</v>
       </c>
     </row>
@@ -1728,7 +1729,7 @@
       <c r="A43" t="n">
         <v>42</v>
       </c>
-      <c r="B43" s="4" t="n">
+      <c r="B43" s="14" t="n">
         <v>45850</v>
       </c>
       <c r="C43" t="inlineStr">
@@ -1746,7 +1747,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F43" s="12" t="n">
+      <c r="F43" t="n">
         <v>20000000</v>
       </c>
     </row>
@@ -1754,7 +1755,7 @@
       <c r="A44" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="11" t="n">
+      <c r="B44" s="14" t="n">
         <v>45851</v>
       </c>
       <c r="C44" t="inlineStr">
@@ -1772,7 +1773,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F44" s="12" t="n">
+      <c r="F44" t="n">
         <v>15700000</v>
       </c>
     </row>
@@ -1780,7 +1781,7 @@
       <c r="A45" t="n">
         <v>44</v>
       </c>
-      <c r="B45" s="11" t="n">
+      <c r="B45" s="14" t="n">
         <v>45861</v>
       </c>
       <c r="C45" t="inlineStr">
@@ -1798,7 +1799,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F45" s="12" t="n">
+      <c r="F45" t="n">
         <v>30000000</v>
       </c>
     </row>
@@ -1806,7 +1807,7 @@
       <c r="A46" t="n">
         <v>45</v>
       </c>
-      <c r="B46" s="11" t="n">
+      <c r="B46" s="14" t="n">
         <v>45861</v>
       </c>
       <c r="C46" t="inlineStr">
@@ -1824,7 +1825,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F46" s="12" t="n">
+      <c r="F46" t="n">
         <v>3680000</v>
       </c>
     </row>
@@ -1832,7 +1833,7 @@
       <c r="A47" t="n">
         <v>46</v>
       </c>
-      <c r="B47" s="11" t="n">
+      <c r="B47" s="14" t="n">
         <v>45861</v>
       </c>
       <c r="C47" t="inlineStr">
@@ -1850,7 +1851,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F47" s="12" t="n">
+      <c r="F47" t="n">
         <v>42000000</v>
       </c>
     </row>
@@ -1858,7 +1859,7 @@
       <c r="A48" t="n">
         <v>47</v>
       </c>
-      <c r="B48" s="11" t="n">
+      <c r="B48" s="14" t="n">
         <v>45861</v>
       </c>
       <c r="C48" t="inlineStr">
@@ -1876,7 +1877,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F48" s="12" t="n">
+      <c r="F48" t="n">
         <v>17000000</v>
       </c>
     </row>
@@ -1884,7 +1885,7 @@
       <c r="A49" t="n">
         <v>48</v>
       </c>
-      <c r="B49" s="11" t="n">
+      <c r="B49" s="14" t="n">
         <v>45870</v>
       </c>
       <c r="C49" t="inlineStr">
@@ -1902,7 +1903,7 @@
           <t>abono</t>
         </is>
       </c>
-      <c r="F49" s="12" t="n">
+      <c r="F49" t="n">
         <v>12000000</v>
       </c>
     </row>
@@ -1910,7 +1911,7 @@
       <c r="A50" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="11" t="n">
+      <c r="B50" s="14" t="n">
         <v>45870</v>
       </c>
       <c r="C50" t="inlineStr">
@@ -1928,7 +1929,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F50" s="12" t="n">
+      <c r="F50" t="n">
         <v>8000000</v>
       </c>
     </row>
@@ -1936,7 +1937,7 @@
       <c r="A51" t="n">
         <v>50</v>
       </c>
-      <c r="B51" s="11" t="n">
+      <c r="B51" s="14" t="n">
         <v>45873</v>
       </c>
       <c r="C51" t="inlineStr">
@@ -1954,7 +1955,7 @@
           <t>Abonos General</t>
         </is>
       </c>
-      <c r="F51" s="12" t="n">
+      <c r="F51" t="n">
         <v>1300000</v>
       </c>
     </row>
@@ -1962,7 +1963,7 @@
       <c r="A52" t="n">
         <v>51</v>
       </c>
-      <c r="B52" s="11" t="n">
+      <c r="B52" s="14" t="n">
         <v>45862</v>
       </c>
       <c r="C52" t="inlineStr">
@@ -1980,7 +1981,7 @@
           <t>Factura</t>
         </is>
       </c>
-      <c r="F52" s="12" t="n">
+      <c r="F52" t="n">
         <v>111361900</v>
       </c>
     </row>
@@ -1988,7 +1989,7 @@
       <c r="A53" t="n">
         <v>52</v>
       </c>
-      <c r="B53" s="11" t="n">
+      <c r="B53" s="14" t="n">
         <v>45864</v>
       </c>
       <c r="C53" t="inlineStr">
@@ -2006,7 +2007,7 @@
           <t>Factura</t>
         </is>
       </c>
-      <c r="F53" s="12" t="n">
+      <c r="F53" t="n">
         <v>54502000</v>
       </c>
     </row>
@@ -2014,7 +2015,7 @@
       <c r="A54" t="n">
         <v>53</v>
       </c>
-      <c r="B54" s="11" t="n">
+      <c r="B54" s="14" t="n">
         <v>45865</v>
       </c>
       <c r="C54" t="inlineStr">
@@ -2032,7 +2033,7 @@
           <t>Factura</t>
         </is>
       </c>
-      <c r="F54" s="12" t="n">
+      <c r="F54" t="n">
         <v>47909300</v>
       </c>
     </row>
@@ -2040,7 +2041,7 @@
       <c r="A55" t="n">
         <v>54</v>
       </c>
-      <c r="B55" s="11" t="n">
+      <c r="B55" s="14" t="n">
         <v>45863</v>
       </c>
       <c r="C55" t="inlineStr">
@@ -2058,7 +2059,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F55" s="12" t="n">
+      <c r="F55" t="n">
         <v>76190000</v>
       </c>
     </row>
@@ -2066,7 +2067,7 @@
       <c r="A56" t="n">
         <v>55</v>
       </c>
-      <c r="B56" s="11" t="n">
+      <c r="B56" s="14" t="n">
         <v>45866</v>
       </c>
       <c r="C56" t="inlineStr">
@@ -2084,7 +2085,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F56" s="12" t="n">
+      <c r="F56" t="n">
         <v>18448000</v>
       </c>
     </row>
@@ -2092,7 +2093,7 @@
       <c r="A57" t="n">
         <v>56</v>
       </c>
-      <c r="B57" s="11" t="n">
+      <c r="B57" s="14" t="n">
         <v>45870</v>
       </c>
       <c r="C57" t="inlineStr">
@@ -2110,7 +2111,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F57" s="12" t="n">
+      <c r="F57" t="n">
         <v>50000000</v>
       </c>
     </row>
@@ -2118,7 +2119,7 @@
       <c r="A58" t="n">
         <v>57</v>
       </c>
-      <c r="B58" s="11" t="n">
+      <c r="B58" s="14" t="n">
         <v>45871</v>
       </c>
       <c r="C58" t="inlineStr">
@@ -2136,7 +2137,7 @@
           <t>Factura</t>
         </is>
       </c>
-      <c r="F58" s="12" t="n">
+      <c r="F58" t="n">
         <v>52311350</v>
       </c>
     </row>
@@ -2144,7 +2145,7 @@
       <c r="A59" t="n">
         <v>58</v>
       </c>
-      <c r="B59" s="11" t="n">
+      <c r="B59" s="14" t="n">
         <v>45871</v>
       </c>
       <c r="C59" t="inlineStr">
@@ -2162,7 +2163,7 @@
           <t>Factura</t>
         </is>
       </c>
-      <c r="F59" s="12" t="n">
+      <c r="F59" t="n">
         <v>46308300</v>
       </c>
     </row>
@@ -2170,7 +2171,7 @@
       <c r="A60" t="n">
         <v>59</v>
       </c>
-      <c r="B60" s="11" t="n">
+      <c r="B60" s="14" t="n">
         <v>45872</v>
       </c>
       <c r="C60" t="inlineStr">
@@ -2188,7 +2189,7 @@
           <t>Factura</t>
         </is>
       </c>
-      <c r="F60" s="12" t="n">
+      <c r="F60" t="n">
         <v>44895800</v>
       </c>
     </row>
@@ -2196,7 +2197,7 @@
       <c r="A61" t="n">
         <v>60</v>
       </c>
-      <c r="B61" s="11" t="n">
+      <c r="B61" s="14" t="n">
         <v>45828</v>
       </c>
       <c r="C61" t="inlineStr">
@@ -2214,7 +2215,7 @@
           <t>Saldo</t>
         </is>
       </c>
-      <c r="F61" s="12" t="n">
+      <c r="F61" t="n">
         <v>24844250</v>
       </c>
     </row>
@@ -2222,7 +2223,7 @@
       <c r="A62" t="n">
         <v>61</v>
       </c>
-      <c r="B62" s="11" t="n">
+      <c r="B62" s="14" t="n">
         <v>45828</v>
       </c>
       <c r="C62" t="inlineStr">
@@ -2240,7 +2241,7 @@
           <t>Factura</t>
         </is>
       </c>
-      <c r="F62" s="12" t="n">
+      <c r="F62" t="n">
         <v>55805400</v>
       </c>
     </row>
@@ -2248,7 +2249,7 @@
       <c r="A63" t="n">
         <v>62</v>
       </c>
-      <c r="B63" s="11" t="n">
+      <c r="B63" s="14" t="n">
         <v>45832</v>
       </c>
       <c r="C63" t="inlineStr">
@@ -2266,7 +2267,7 @@
           <t>Factura</t>
         </is>
       </c>
-      <c r="F63" s="12" t="n">
+      <c r="F63" t="n">
         <v>62911450</v>
       </c>
     </row>
@@ -2274,7 +2275,7 @@
       <c r="A64" t="n">
         <v>63</v>
       </c>
-      <c r="B64" s="11" t="n">
+      <c r="B64" s="14" t="n">
         <v>45832</v>
       </c>
       <c r="C64" t="inlineStr">
@@ -2292,7 +2293,7 @@
           <t>Factura</t>
         </is>
       </c>
-      <c r="F64" s="12" t="n">
+      <c r="F64" t="n">
         <v>57171000</v>
       </c>
     </row>
@@ -2300,7 +2301,7 @@
       <c r="A65" t="n">
         <v>64</v>
       </c>
-      <c r="B65" s="11" t="n">
+      <c r="B65" s="14" t="n">
         <v>45820</v>
       </c>
       <c r="C65" t="inlineStr">
@@ -2318,7 +2319,7 @@
           <t>Factura</t>
         </is>
       </c>
-      <c r="F65" s="12" t="n">
+      <c r="F65" t="n">
         <v>57454850</v>
       </c>
     </row>
@@ -2326,7 +2327,7 @@
       <c r="A66" t="n">
         <v>65</v>
       </c>
-      <c r="B66" s="11" t="n">
+      <c r="B66" s="14" t="n">
         <v>45867</v>
       </c>
       <c r="C66" t="inlineStr">
@@ -2344,7 +2345,7 @@
           <t>Factura</t>
         </is>
       </c>
-      <c r="F66" s="12" t="n">
+      <c r="F66" t="n">
         <v>54618600</v>
       </c>
     </row>
@@ -2352,7 +2353,7 @@
       <c r="A67" t="n">
         <v>66</v>
       </c>
-      <c r="B67" s="11" t="n">
+      <c r="B67" s="14" t="n">
         <v>45867</v>
       </c>
       <c r="C67" t="inlineStr">
@@ -2370,7 +2371,7 @@
           <t>Factura</t>
         </is>
       </c>
-      <c r="F67" s="12" t="n">
+      <c r="F67" t="n">
         <v>59959200</v>
       </c>
     </row>
@@ -2378,7 +2379,7 @@
       <c r="A68" t="n">
         <v>67</v>
       </c>
-      <c r="B68" s="11" t="n">
+      <c r="B68" s="14" t="n">
         <v>45867</v>
       </c>
       <c r="C68" t="inlineStr">
@@ -2396,7 +2397,7 @@
           <t>Factura</t>
         </is>
       </c>
-      <c r="F68" s="12" t="n">
+      <c r="F68" t="n">
         <v>58144600</v>
       </c>
     </row>
@@ -2404,7 +2405,7 @@
       <c r="A69" t="n">
         <v>68</v>
       </c>
-      <c r="B69" s="11" t="n">
+      <c r="B69" s="14" t="n">
         <v>45867</v>
       </c>
       <c r="C69" t="inlineStr">
@@ -2422,7 +2423,7 @@
           <t>Factura</t>
         </is>
       </c>
-      <c r="F69" s="12" t="n">
+      <c r="F69" t="n">
         <v>52584500</v>
       </c>
     </row>
@@ -2430,7 +2431,7 @@
       <c r="A70" t="n">
         <v>69</v>
       </c>
-      <c r="B70" s="11" t="n">
+      <c r="B70" s="14" t="n">
         <v>45867</v>
       </c>
       <c r="C70" t="inlineStr">
@@ -2448,7 +2449,7 @@
           <t>Factura</t>
         </is>
       </c>
-      <c r="F70" s="12" t="n">
+      <c r="F70" t="n">
         <v>50591000</v>
       </c>
     </row>
@@ -2456,7 +2457,7 @@
       <c r="A71" t="n">
         <v>70</v>
       </c>
-      <c r="B71" s="11" t="n">
+      <c r="B71" s="14" t="n">
         <v>45827</v>
       </c>
       <c r="C71" t="inlineStr">
@@ -2474,7 +2475,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F71" s="12" t="n">
+      <c r="F71" t="n">
         <v>33000000</v>
       </c>
     </row>
@@ -2482,7 +2483,7 @@
       <c r="A72" t="n">
         <v>71</v>
       </c>
-      <c r="B72" s="11" t="n">
+      <c r="B72" s="14" t="n">
         <v>45832</v>
       </c>
       <c r="C72" t="inlineStr">
@@ -2500,7 +2501,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F72" s="12" t="n">
+      <c r="F72" t="n">
         <v>50000000</v>
       </c>
     </row>
@@ -2508,7 +2509,7 @@
       <c r="A73" t="n">
         <v>72</v>
       </c>
-      <c r="B73" s="11" t="n">
+      <c r="B73" s="14" t="n">
         <v>45839</v>
       </c>
       <c r="C73" t="inlineStr">
@@ -2526,7 +2527,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F73" s="12" t="n">
+      <c r="F73" t="n">
         <v>13106000</v>
       </c>
     </row>
@@ -2534,7 +2535,7 @@
       <c r="A74" t="n">
         <v>73</v>
       </c>
-      <c r="B74" s="11" t="n">
+      <c r="B74" s="14" t="n">
         <v>45839</v>
       </c>
       <c r="C74" t="inlineStr">
@@ -2552,7 +2553,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F74" s="12" t="n">
+      <c r="F74" t="n">
         <v>16894000</v>
       </c>
     </row>
@@ -2560,7 +2561,7 @@
       <c r="A75" t="n">
         <v>74</v>
       </c>
-      <c r="B75" s="11" t="n">
+      <c r="B75" s="14" t="n">
         <v>45848</v>
       </c>
       <c r="C75" t="inlineStr">
@@ -2578,7 +2579,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F75" s="12" t="n">
+      <c r="F75" t="n">
         <v>30000000</v>
       </c>
     </row>
@@ -2586,7 +2587,7 @@
       <c r="A76" t="n">
         <v>75</v>
       </c>
-      <c r="B76" s="11" t="n">
+      <c r="B76" s="14" t="n">
         <v>45849</v>
       </c>
       <c r="C76" t="inlineStr">
@@ -2604,7 +2605,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F76" s="12" t="n">
+      <c r="F76" t="n">
         <v>30000000</v>
       </c>
     </row>
@@ -2612,7 +2613,7 @@
       <c r="A77" t="n">
         <v>76</v>
       </c>
-      <c r="B77" s="11" t="n">
+      <c r="B77" s="14" t="n">
         <v>45860</v>
       </c>
       <c r="C77" t="inlineStr">
@@ -2630,7 +2631,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F77" s="12" t="n">
+      <c r="F77" t="n">
         <v>25000000</v>
       </c>
     </row>
@@ -2638,7 +2639,7 @@
       <c r="A78" t="n">
         <v>77</v>
       </c>
-      <c r="B78" s="11" t="n">
+      <c r="B78" s="14" t="n">
         <v>45867</v>
       </c>
       <c r="C78" t="inlineStr">
@@ -2656,7 +2657,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F78" s="12" t="n">
+      <c r="F78" t="n">
         <v>25000000</v>
       </c>
     </row>
@@ -2664,7 +2665,7 @@
       <c r="A79" t="n">
         <v>78</v>
       </c>
-      <c r="B79" s="11" t="n">
+      <c r="B79" s="14" t="n">
         <v>45867</v>
       </c>
       <c r="C79" t="inlineStr">
@@ -2682,7 +2683,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F79" s="12" t="n">
+      <c r="F79" t="n">
         <v>13750000</v>
       </c>
     </row>
@@ -2690,7 +2691,7 @@
       <c r="A80" t="n">
         <v>79</v>
       </c>
-      <c r="B80" s="11" t="n">
+      <c r="B80" s="14" t="n">
         <v>45867</v>
       </c>
       <c r="C80" t="inlineStr">
@@ -2708,7 +2709,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F80" s="12" t="n">
+      <c r="F80" t="n">
         <v>36200000</v>
       </c>
     </row>
@@ -2716,7 +2717,7 @@
       <c r="A81" t="n">
         <v>80</v>
       </c>
-      <c r="B81" s="11" t="n">
+      <c r="B81" s="14" t="n">
         <v>45868</v>
       </c>
       <c r="C81" t="inlineStr">
@@ -2734,7 +2735,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F81" s="12" t="n">
+      <c r="F81" t="n">
         <v>40000000</v>
       </c>
     </row>
@@ -2742,7 +2743,7 @@
       <c r="A82" t="n">
         <v>81</v>
       </c>
-      <c r="B82" s="11" t="n">
+      <c r="B82" s="14" t="n">
         <v>45870</v>
       </c>
       <c r="C82" t="inlineStr">
@@ -2760,7 +2761,7 @@
           <t>Abono</t>
         </is>
       </c>
-      <c r="F82" s="12" t="n">
+      <c r="F82" t="n">
         <v>50000000</v>
       </c>
     </row>
@@ -2768,7 +2769,7 @@
       <c r="A83" t="n">
         <v>82</v>
       </c>
-      <c r="B83" s="13" t="n">
+      <c r="B83" s="14" t="n">
         <v>45877</v>
       </c>
       <c r="C83" t="inlineStr">
@@ -4458,7 +4459,7 @@
       <c r="A148" t="n">
         <v>147</v>
       </c>
-      <c r="B148" s="13" t="n">
+      <c r="B148" s="14" t="n">
         <v>45860</v>
       </c>
       <c r="C148" t="inlineStr">
@@ -4478,6 +4479,136 @@
       </c>
       <c r="F148" t="n">
         <v>57654400</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>148</v>
+      </c>
+      <c r="B149" s="14" t="n">
+        <v>45900</v>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Pepito</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="F149" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>149</v>
+      </c>
+      <c r="B150" s="14" t="n">
+        <v>45900</v>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Pepito</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Ahorro</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F150" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>150</v>
+      </c>
+      <c r="B151" s="14" t="n">
+        <v>45900</v>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Pepito</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Ahorro</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F151" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>151</v>
+      </c>
+      <c r="B152" s="14" t="n">
+        <v>45900</v>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Pepito</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Ahorro</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F152" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>152</v>
+      </c>
+      <c r="B153" s="15" t="n">
+        <v>45893</v>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Prueba 3</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Ahorro</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="F153" t="n">
+        <v>50000</v>
       </c>
     </row>
   </sheetData>
@@ -4494,136 +4625,197 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col width="21" customWidth="1" min="1" max="1"/>
-    <col width="17.109375" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="15.33203125" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="15" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="17.109375" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="15.33203125" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="15" bestFit="1" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
+        <is>
+          <t>Id</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Proveedor</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Total Facturas</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Total Ahorro</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Saldo</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Sergio Garcia</t>
-        </is>
-      </c>
-      <c r="B2" s="12" t="n">
+      <c r="A2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Sergio Garcia</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>622195050</v>
       </c>
-      <c r="C2" s="12" t="n">
+      <c r="D2" t="n">
         <v>570802868</v>
       </c>
-      <c r="D2" s="12" t="n">
+      <c r="E2" t="n">
         <v>51392182</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>13</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Jorge Trabadiya</t>
         </is>
       </c>
-      <c r="B3" s="12" t="n">
+      <c r="C3" t="n">
         <v>357288650</v>
       </c>
-      <c r="C3" s="12" t="n">
+      <c r="D3" t="n">
         <v>265278500</v>
       </c>
-      <c r="D3" s="12" t="n">
+      <c r="E3" t="n">
         <v>92010150</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>13</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Ramiro</t>
         </is>
       </c>
-      <c r="B4" s="12" t="n">
+      <c r="C4" t="n">
         <v>591739250</v>
       </c>
-      <c r="C4" s="12" t="n">
+      <c r="D4" t="n">
         <v>385550000</v>
       </c>
-      <c r="D4" s="12" t="n">
+      <c r="E4" t="n">
         <v>206189250</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" t="n">
+        <v>13</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Fernando Guaza</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>388594900</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>433900000</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>-45305100</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" t="n">
+        <v>13</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Rey</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>648442750</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>572564600</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>75878150</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" t="n">
+        <v>13</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>Jonathan Guaza</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>204357400</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>139386000</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>64971400</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>13</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Pepito</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>60000</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-10000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>13</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Prueba 3</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>50000</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-50000</v>
       </c>
     </row>
   </sheetData>
@@ -4642,8 +4834,8 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -4654,27 +4846,27 @@
           <t>Id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">Fecha </t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>Proveedor</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>Detalle</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>Observación</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -4684,7 +4876,7 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="n">
+      <c r="B2" s="13" t="n">
         <v>45880</v>
       </c>
       <c r="C2" t="inlineStr">
@@ -4718,10 +4910,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -4729,38 +4921,46 @@
     <row r="1" ht="28.8" customHeight="1">
       <c r="A1" s="8" t="inlineStr">
         <is>
+          <t>Id</t>
+        </is>
+      </c>
+      <c r="B1" s="8" t="inlineStr">
+        <is>
           <t>Proveedor</t>
         </is>
       </c>
-      <c r="B1" s="9" t="inlineStr">
+      <c r="C1" s="9" t="inlineStr">
         <is>
           <t>Total Facturas</t>
         </is>
       </c>
-      <c r="C1" s="9" t="inlineStr">
+      <c r="D1" s="9" t="inlineStr">
         <is>
           <t>Total Ahorro</t>
         </is>
       </c>
-      <c r="D1" s="10" t="inlineStr">
+      <c r="E1" s="10" t="inlineStr">
         <is>
           <t>Saldo</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>Pepito</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>50000000</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>0</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>50000000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Visualizacion de celular y doble copia
</commit_message>
<xml_diff>
--- a/Financiero.xlsx
+++ b/Financiero.xlsx
@@ -614,7 +614,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F153"/>
+  <dimension ref="A1:F154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:F1"/>
@@ -4589,7 +4589,7 @@
       <c r="A153" t="n">
         <v>152</v>
       </c>
-      <c r="B153" s="15" t="n">
+      <c r="B153" s="14" t="n">
         <v>45893</v>
       </c>
       <c r="C153" t="inlineStr">
@@ -4608,6 +4608,32 @@
         </is>
       </c>
       <c r="F153" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>153</v>
+      </c>
+      <c r="B154" s="15" t="n">
+        <v>45901</v>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Prueba 3</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Ahorro</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F154" t="n">
         <v>50000</v>
       </c>
     </row>
@@ -4668,7 +4694,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -4687,7 +4713,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -4706,7 +4732,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -4725,7 +4751,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -4744,7 +4770,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -4763,7 +4789,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -4782,7 +4808,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -4801,7 +4827,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -4812,10 +4838,10 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="E9" t="n">
-        <v>-50000</v>
+        <v>-100000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mejoras en diseño y nuevas funcionalidades
</commit_message>
<xml_diff>
--- a/Financiero.xlsx
+++ b/Financiero.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Proveedores" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Resumen" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ProveedoresCliente" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ResumenCliente" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Gastos" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -18,14 +19,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00;\-&quot;$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="167" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="168" formatCode="yyyy-mm-dd h:mm:ss"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="1">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -33,38 +31,16 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color theme="0"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor theme="4"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -72,127 +48,19 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="4" tint="0.3999755851924192"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.3999755851924192"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.3999755851924192"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.3999755851924192"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.3999755851924192"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.3999755851924192"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.3999755851924192"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.3999755851924192"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <numFmt numFmtId="11" formatCode="&quot;$&quot;\ #,##0.00;\-&quot;$&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="11" formatCode="&quot;$&quot;\ #,##0.00;\-&quot;$&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <b val="1"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <condense val="0"/>
-        <color theme="1"/>
-        <extend val="0"/>
-        <sz val="11"/>
-        <vertAlign val="baseline"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="11" formatCode="&quot;$&quot;\ #,##0.00;\-&quot;$&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <b val="1"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <condense val="0"/>
-        <color theme="1"/>
-        <extend val="0"/>
-        <sz val="11"/>
-        <vertAlign val="baseline"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </dxf>
-  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -263,33 +131,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Proveedor4" displayName="Proveedor4" ref="B1:F82" headerRowCount="1" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="B1:F82"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Fecha " dataDxfId="4"/>
-    <tableColumn id="2" name="Proveedor"/>
-    <tableColumn id="3" name="Detalle"/>
-    <tableColumn id="4" name="Observación"/>
-    <tableColumn id="5" name="Total" dataDxfId="3"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Resumen" displayName="Resumen" ref="B1:E7" headerRowCount="1" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="B1:E7"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Proveedor"/>
-    <tableColumn id="2" name="Total Facturas" dataDxfId="1"/>
-    <tableColumn id="3" name="Total Abonos"/>
-    <tableColumn id="4" name="Saldo" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -609,25 +450,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Hoja1">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F148"/>
+  <dimension ref="A1:H157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col width="11.5546875" customWidth="1" style="4" min="2" max="2"/>
-    <col width="13.33203125" customWidth="1" min="5" max="5"/>
-    <col width="24.21875" customWidth="1" min="6" max="6"/>
+    <col width="20.109375" customWidth="1" style="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Id</t>
         </is>
@@ -637,24 +476,34 @@
           <t>Fecha</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Proveedor</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Detalle</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Obs</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Total</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>IdFactura</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Estado</t>
         </is>
       </c>
     </row>
@@ -662,7 +511,7 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="n">
+      <c r="B2" s="2" t="n">
         <v>45816</v>
       </c>
       <c r="C2" t="inlineStr">
@@ -682,13 +531,23 @@
       </c>
       <c r="F2" t="n">
         <v>52433000</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="n">
+      <c r="B3" s="2" t="n">
         <v>45816</v>
       </c>
       <c r="C3" t="inlineStr">
@@ -708,13 +567,23 @@
       </c>
       <c r="F3" t="n">
         <v>26354000</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="n">
+      <c r="B4" s="2" t="n">
         <v>45818</v>
       </c>
       <c r="C4" t="inlineStr">
@@ -734,13 +603,23 @@
       </c>
       <c r="F4" t="n">
         <v>19129000</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="n">
+      <c r="B5" s="2" t="n">
         <v>45820</v>
       </c>
       <c r="C5" t="inlineStr">
@@ -760,13 +639,23 @@
       </c>
       <c r="F5" t="n">
         <v>54840000</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="n">
+      <c r="B6" s="2" t="n">
         <v>45828</v>
       </c>
       <c r="C6" t="inlineStr">
@@ -786,13 +675,23 @@
       </c>
       <c r="F6" t="n">
         <v>63918000</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="n">
+      <c r="B7" s="2" t="n">
         <v>45843</v>
       </c>
       <c r="C7" t="inlineStr">
@@ -812,13 +711,23 @@
       </c>
       <c r="F7" t="n">
         <v>136060000</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="12" t="n">
+      <c r="B8" s="2" t="n">
         <v>45848</v>
       </c>
       <c r="C8" t="inlineStr">
@@ -838,13 +747,23 @@
       </c>
       <c r="F8" t="n">
         <v>98794250</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="12" t="n">
+      <c r="B9" s="2" t="n">
         <v>45849</v>
       </c>
       <c r="C9" t="inlineStr">
@@ -864,13 +783,23 @@
       </c>
       <c r="F9" t="n">
         <v>44541000</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="12" t="n">
+      <c r="B10" s="2" t="n">
         <v>45863</v>
       </c>
       <c r="C10" t="inlineStr">
@@ -890,13 +819,23 @@
       </c>
       <c r="F10" t="n">
         <v>126125800</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="12" t="n">
+      <c r="B11" s="2" t="n">
         <v>45807</v>
       </c>
       <c r="C11" t="inlineStr">
@@ -916,13 +855,23 @@
       </c>
       <c r="F11" t="n">
         <v>13828960</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="12" t="n">
+      <c r="B12" s="2" t="n">
         <v>45807</v>
       </c>
       <c r="C12" t="inlineStr">
@@ -942,13 +891,23 @@
       </c>
       <c r="F12" t="n">
         <v>26554608</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="12" t="n">
+      <c r="B13" s="2" t="n">
         <v>45722</v>
       </c>
       <c r="C13" t="inlineStr">
@@ -968,13 +927,23 @@
       </c>
       <c r="F13" t="n">
         <v>12050000</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="12" t="n">
+      <c r="B14" s="2" t="n">
         <v>45819</v>
       </c>
       <c r="C14" t="inlineStr">
@@ -994,13 +963,23 @@
       </c>
       <c r="F14" t="n">
         <v>45000000</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="12" t="n">
+      <c r="B15" s="2" t="n">
         <v>45820</v>
       </c>
       <c r="C15" t="inlineStr">
@@ -1020,13 +999,23 @@
       </c>
       <c r="F15" t="n">
         <v>9000000</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="12" t="n">
+      <c r="B16" s="2" t="n">
         <v>45822</v>
       </c>
       <c r="C16" t="inlineStr">
@@ -1046,13 +1035,23 @@
       </c>
       <c r="F16" t="n">
         <v>5994800</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="12" t="n">
+      <c r="B17" s="2" t="n">
         <v>45822</v>
       </c>
       <c r="C17" t="inlineStr">
@@ -1072,13 +1071,23 @@
       </c>
       <c r="F17" t="n">
         <v>5341300</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="12" t="n">
+      <c r="B18" s="2" t="n">
         <v>45822</v>
       </c>
       <c r="C18" t="inlineStr">
@@ -1098,13 +1107,23 @@
       </c>
       <c r="F18" t="n">
         <v>18976000</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="12" t="n">
+      <c r="B19" s="2" t="n">
         <v>45829</v>
       </c>
       <c r="C19" t="inlineStr">
@@ -1124,13 +1143,23 @@
       </c>
       <c r="F19" t="n">
         <v>10000000</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="12" t="n">
+      <c r="B20" s="2" t="n">
         <v>45833</v>
       </c>
       <c r="C20" t="inlineStr">
@@ -1150,13 +1179,23 @@
       </c>
       <c r="F20" t="n">
         <v>10000000</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="12" t="n">
+      <c r="B21" s="2" t="n">
         <v>45836</v>
       </c>
       <c r="C21" t="inlineStr">
@@ -1176,13 +1215,23 @@
       </c>
       <c r="F21" t="n">
         <v>10000000</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="12" t="n">
+      <c r="B22" s="2" t="n">
         <v>45839</v>
       </c>
       <c r="C22" t="inlineStr">
@@ -1202,13 +1251,23 @@
       </c>
       <c r="F22" t="n">
         <v>20000000</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="12" t="n">
+      <c r="B23" s="2" t="n">
         <v>45839</v>
       </c>
       <c r="C23" t="inlineStr">
@@ -1228,13 +1287,23 @@
       </c>
       <c r="F23" t="n">
         <v>10000000</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="12" t="n">
+      <c r="B24" s="2" t="n">
         <v>45839</v>
       </c>
       <c r="C24" t="inlineStr">
@@ -1254,13 +1323,23 @@
       </c>
       <c r="F24" t="n">
         <v>4000000</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="12" t="n">
+      <c r="B25" s="2" t="n">
         <v>45839</v>
       </c>
       <c r="C25" t="inlineStr">
@@ -1280,13 +1359,23 @@
       </c>
       <c r="F25" t="n">
         <v>18500000</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="12" t="n">
+      <c r="B26" s="2" t="n">
         <v>45840</v>
       </c>
       <c r="C26" t="inlineStr">
@@ -1306,13 +1395,23 @@
       </c>
       <c r="F26" t="n">
         <v>10000000</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="12" t="n">
+      <c r="B27" s="2" t="n">
         <v>45840</v>
       </c>
       <c r="C27" t="inlineStr">
@@ -1332,13 +1431,23 @@
       </c>
       <c r="F27" t="n">
         <v>10089200</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="12" t="n">
+      <c r="B28" s="2" t="n">
         <v>45840</v>
       </c>
       <c r="C28" t="inlineStr">
@@ -1358,13 +1467,23 @@
       </c>
       <c r="F28" t="n">
         <v>16994000</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="12" t="n">
+      <c r="B29" s="2" t="n">
         <v>45841</v>
       </c>
       <c r="C29" t="inlineStr">
@@ -1384,13 +1503,23 @@
       </c>
       <c r="F29" t="n">
         <v>5500000</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="12" t="n">
+      <c r="B30" s="2" t="n">
         <v>45841</v>
       </c>
       <c r="C30" t="inlineStr">
@@ -1410,13 +1539,23 @@
       </c>
       <c r="F30" t="n">
         <v>6000000</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="12" t="n">
+      <c r="B31" s="2" t="n">
         <v>45841</v>
       </c>
       <c r="C31" t="inlineStr">
@@ -1436,13 +1575,23 @@
       </c>
       <c r="F31" t="n">
         <v>4000000</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="12" t="n">
+      <c r="B32" s="2" t="n">
         <v>45841</v>
       </c>
       <c r="C32" t="inlineStr">
@@ -1462,13 +1611,23 @@
       </c>
       <c r="F32" t="n">
         <v>14064000</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="12" t="n">
+      <c r="B33" s="2" t="n">
         <v>45841</v>
       </c>
       <c r="C33" t="inlineStr">
@@ -1488,13 +1647,23 @@
       </c>
       <c r="F33" t="n">
         <v>19450000</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="12" t="n">
+      <c r="B34" s="2" t="n">
         <v>45842</v>
       </c>
       <c r="C34" t="inlineStr">
@@ -1514,13 +1683,23 @@
       </c>
       <c r="F34" t="n">
         <v>22000000</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="12" t="n">
+      <c r="B35" s="2" t="n">
         <v>45847</v>
       </c>
       <c r="C35" t="inlineStr">
@@ -1540,13 +1719,23 @@
       </c>
       <c r="F35" t="n">
         <v>17000000</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="12" t="n">
+      <c r="B36" s="2" t="n">
         <v>45847</v>
       </c>
       <c r="C36" t="inlineStr">
@@ -1566,13 +1755,23 @@
       </c>
       <c r="F36" t="n">
         <v>3000000</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="12" t="n">
+      <c r="B37" s="2" t="n">
         <v>45847</v>
       </c>
       <c r="C37" t="inlineStr">
@@ -1592,13 +1791,23 @@
       </c>
       <c r="F37" t="n">
         <v>3000000</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="12" t="n">
+      <c r="B38" s="2" t="n">
         <v>45847</v>
       </c>
       <c r="C38" t="inlineStr">
@@ -1618,13 +1827,23 @@
       </c>
       <c r="F38" t="n">
         <v>1480000</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="12" t="n">
+      <c r="B39" s="2" t="n">
         <v>45847</v>
       </c>
       <c r="C39" t="inlineStr">
@@ -1644,13 +1863,23 @@
       </c>
       <c r="F39" t="n">
         <v>2133000</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="12" t="n">
+      <c r="B40" s="2" t="n">
         <v>45847</v>
       </c>
       <c r="C40" t="inlineStr">
@@ -1670,13 +1899,23 @@
       </c>
       <c r="F40" t="n">
         <v>3000000</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="12" t="n">
+      <c r="B41" s="2" t="n">
         <v>45847</v>
       </c>
       <c r="C41" t="inlineStr">
@@ -1696,13 +1935,23 @@
       </c>
       <c r="F41" t="n">
         <v>80000</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
         <v>41</v>
       </c>
-      <c r="B42" s="12" t="n">
+      <c r="B42" s="2" t="n">
         <v>45847</v>
       </c>
       <c r="C42" t="inlineStr">
@@ -1722,13 +1971,23 @@
       </c>
       <c r="F42" t="n">
         <v>64087000</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
         <v>42</v>
       </c>
-      <c r="B43" s="12" t="n">
+      <c r="B43" s="2" t="n">
         <v>45850</v>
       </c>
       <c r="C43" t="inlineStr">
@@ -1748,13 +2007,23 @@
       </c>
       <c r="F43" t="n">
         <v>20000000</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="12" t="n">
+      <c r="B44" s="2" t="n">
         <v>45851</v>
       </c>
       <c r="C44" t="inlineStr">
@@ -1774,13 +2043,23 @@
       </c>
       <c r="F44" t="n">
         <v>15700000</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
         <v>44</v>
       </c>
-      <c r="B45" s="12" t="n">
+      <c r="B45" s="2" t="n">
         <v>45861</v>
       </c>
       <c r="C45" t="inlineStr">
@@ -1800,13 +2079,23 @@
       </c>
       <c r="F45" t="n">
         <v>30000000</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
         <v>45</v>
       </c>
-      <c r="B46" s="12" t="n">
+      <c r="B46" s="2" t="n">
         <v>45861</v>
       </c>
       <c r="C46" t="inlineStr">
@@ -1826,13 +2115,23 @@
       </c>
       <c r="F46" t="n">
         <v>3680000</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
         <v>46</v>
       </c>
-      <c r="B47" s="12" t="n">
+      <c r="B47" s="2" t="n">
         <v>45861</v>
       </c>
       <c r="C47" t="inlineStr">
@@ -1852,13 +2151,23 @@
       </c>
       <c r="F47" t="n">
         <v>42000000</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
         <v>47</v>
       </c>
-      <c r="B48" s="12" t="n">
+      <c r="B48" s="2" t="n">
         <v>45861</v>
       </c>
       <c r="C48" t="inlineStr">
@@ -1878,13 +2187,23 @@
       </c>
       <c r="F48" t="n">
         <v>17000000</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
         <v>48</v>
       </c>
-      <c r="B49" s="12" t="n">
+      <c r="B49" s="2" t="n">
         <v>45870</v>
       </c>
       <c r="C49" t="inlineStr">
@@ -1904,13 +2223,23 @@
       </c>
       <c r="F49" t="n">
         <v>12000000</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="12" t="n">
+      <c r="B50" s="2" t="n">
         <v>45870</v>
       </c>
       <c r="C50" t="inlineStr">
@@ -1930,13 +2259,23 @@
       </c>
       <c r="F50" t="n">
         <v>8000000</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
         <v>50</v>
       </c>
-      <c r="B51" s="12" t="n">
+      <c r="B51" s="2" t="n">
         <v>45873</v>
       </c>
       <c r="C51" t="inlineStr">
@@ -1956,13 +2295,23 @@
       </c>
       <c r="F51" t="n">
         <v>1300000</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
         <v>51</v>
       </c>
-      <c r="B52" s="12" t="n">
+      <c r="B52" s="2" t="n">
         <v>45862</v>
       </c>
       <c r="C52" t="inlineStr">
@@ -1982,13 +2331,23 @@
       </c>
       <c r="F52" t="n">
         <v>111361900</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
         <v>52</v>
       </c>
-      <c r="B53" s="12" t="n">
+      <c r="B53" s="2" t="n">
         <v>45864</v>
       </c>
       <c r="C53" t="inlineStr">
@@ -2008,13 +2367,23 @@
       </c>
       <c r="F53" t="n">
         <v>54502000</v>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
         <v>53</v>
       </c>
-      <c r="B54" s="12" t="n">
+      <c r="B54" s="2" t="n">
         <v>45865</v>
       </c>
       <c r="C54" t="inlineStr">
@@ -2034,13 +2403,23 @@
       </c>
       <c r="F54" t="n">
         <v>47909300</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
         <v>54</v>
       </c>
-      <c r="B55" s="12" t="n">
+      <c r="B55" s="2" t="n">
         <v>45863</v>
       </c>
       <c r="C55" t="inlineStr">
@@ -2060,13 +2439,23 @@
       </c>
       <c r="F55" t="n">
         <v>76190000</v>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
         <v>55</v>
       </c>
-      <c r="B56" s="12" t="n">
+      <c r="B56" s="2" t="n">
         <v>45866</v>
       </c>
       <c r="C56" t="inlineStr">
@@ -2086,13 +2475,23 @@
       </c>
       <c r="F56" t="n">
         <v>18448000</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
         <v>56</v>
       </c>
-      <c r="B57" s="12" t="n">
+      <c r="B57" s="2" t="n">
         <v>45870</v>
       </c>
       <c r="C57" t="inlineStr">
@@ -2112,13 +2511,23 @@
       </c>
       <c r="F57" t="n">
         <v>50000000</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
         <v>57</v>
       </c>
-      <c r="B58" s="12" t="n">
+      <c r="B58" s="2" t="n">
         <v>45871</v>
       </c>
       <c r="C58" t="inlineStr">
@@ -2138,13 +2547,23 @@
       </c>
       <c r="F58" t="n">
         <v>52311350</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
         <v>58</v>
       </c>
-      <c r="B59" s="12" t="n">
+      <c r="B59" s="2" t="n">
         <v>45871</v>
       </c>
       <c r="C59" t="inlineStr">
@@ -2164,13 +2583,23 @@
       </c>
       <c r="F59" t="n">
         <v>46308300</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
         <v>59</v>
       </c>
-      <c r="B60" s="12" t="n">
+      <c r="B60" s="2" t="n">
         <v>45872</v>
       </c>
       <c r="C60" t="inlineStr">
@@ -2190,13 +2619,23 @@
       </c>
       <c r="F60" t="n">
         <v>44895800</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
         <v>60</v>
       </c>
-      <c r="B61" s="12" t="n">
+      <c r="B61" s="2" t="n">
         <v>45828</v>
       </c>
       <c r="C61" t="inlineStr">
@@ -2216,13 +2655,23 @@
       </c>
       <c r="F61" t="n">
         <v>24844250</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
         <v>61</v>
       </c>
-      <c r="B62" s="12" t="n">
+      <c r="B62" s="2" t="n">
         <v>45828</v>
       </c>
       <c r="C62" t="inlineStr">
@@ -2242,13 +2691,23 @@
       </c>
       <c r="F62" t="n">
         <v>55805400</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
         <v>62</v>
       </c>
-      <c r="B63" s="12" t="n">
+      <c r="B63" s="2" t="n">
         <v>45832</v>
       </c>
       <c r="C63" t="inlineStr">
@@ -2268,13 +2727,23 @@
       </c>
       <c r="F63" t="n">
         <v>62911450</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
         <v>63</v>
       </c>
-      <c r="B64" s="12" t="n">
+      <c r="B64" s="2" t="n">
         <v>45832</v>
       </c>
       <c r="C64" t="inlineStr">
@@ -2294,13 +2763,23 @@
       </c>
       <c r="F64" t="n">
         <v>57171000</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
         <v>64</v>
       </c>
-      <c r="B65" s="12" t="n">
+      <c r="B65" s="2" t="n">
         <v>45820</v>
       </c>
       <c r="C65" t="inlineStr">
@@ -2320,13 +2799,23 @@
       </c>
       <c r="F65" t="n">
         <v>57454850</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
         <v>65</v>
       </c>
-      <c r="B66" s="12" t="n">
+      <c r="B66" s="2" t="n">
         <v>45867</v>
       </c>
       <c r="C66" t="inlineStr">
@@ -2346,13 +2835,23 @@
       </c>
       <c r="F66" t="n">
         <v>54618600</v>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
         <v>66</v>
       </c>
-      <c r="B67" s="12" t="n">
+      <c r="B67" s="2" t="n">
         <v>45867</v>
       </c>
       <c r="C67" t="inlineStr">
@@ -2372,13 +2871,23 @@
       </c>
       <c r="F67" t="n">
         <v>59959200</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
         <v>67</v>
       </c>
-      <c r="B68" s="12" t="n">
+      <c r="B68" s="2" t="n">
         <v>45867</v>
       </c>
       <c r="C68" t="inlineStr">
@@ -2398,13 +2907,23 @@
       </c>
       <c r="F68" t="n">
         <v>58144600</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
         <v>68</v>
       </c>
-      <c r="B69" s="12" t="n">
+      <c r="B69" s="2" t="n">
         <v>45867</v>
       </c>
       <c r="C69" t="inlineStr">
@@ -2424,13 +2943,23 @@
       </c>
       <c r="F69" t="n">
         <v>52584500</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
         <v>69</v>
       </c>
-      <c r="B70" s="12" t="n">
+      <c r="B70" s="2" t="n">
         <v>45867</v>
       </c>
       <c r="C70" t="inlineStr">
@@ -2450,13 +2979,23 @@
       </c>
       <c r="F70" t="n">
         <v>50591000</v>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
         <v>70</v>
       </c>
-      <c r="B71" s="12" t="n">
+      <c r="B71" s="2" t="n">
         <v>45827</v>
       </c>
       <c r="C71" t="inlineStr">
@@ -2476,13 +3015,23 @@
       </c>
       <c r="F71" t="n">
         <v>33000000</v>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
         <v>71</v>
       </c>
-      <c r="B72" s="12" t="n">
+      <c r="B72" s="2" t="n">
         <v>45832</v>
       </c>
       <c r="C72" t="inlineStr">
@@ -2502,13 +3051,23 @@
       </c>
       <c r="F72" t="n">
         <v>50000000</v>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
         <v>72</v>
       </c>
-      <c r="B73" s="12" t="n">
+      <c r="B73" s="2" t="n">
         <v>45839</v>
       </c>
       <c r="C73" t="inlineStr">
@@ -2528,13 +3087,23 @@
       </c>
       <c r="F73" t="n">
         <v>13106000</v>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
         <v>73</v>
       </c>
-      <c r="B74" s="12" t="n">
+      <c r="B74" s="2" t="n">
         <v>45839</v>
       </c>
       <c r="C74" t="inlineStr">
@@ -2554,13 +3123,23 @@
       </c>
       <c r="F74" t="n">
         <v>16894000</v>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
         <v>74</v>
       </c>
-      <c r="B75" s="12" t="n">
+      <c r="B75" s="2" t="n">
         <v>45848</v>
       </c>
       <c r="C75" t="inlineStr">
@@ -2580,13 +3159,23 @@
       </c>
       <c r="F75" t="n">
         <v>30000000</v>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
         <v>75</v>
       </c>
-      <c r="B76" s="12" t="n">
+      <c r="B76" s="2" t="n">
         <v>45849</v>
       </c>
       <c r="C76" t="inlineStr">
@@ -2606,13 +3195,23 @@
       </c>
       <c r="F76" t="n">
         <v>30000000</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
         <v>76</v>
       </c>
-      <c r="B77" s="12" t="n">
+      <c r="B77" s="2" t="n">
         <v>45860</v>
       </c>
       <c r="C77" t="inlineStr">
@@ -2632,13 +3231,23 @@
       </c>
       <c r="F77" t="n">
         <v>25000000</v>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
         <v>77</v>
       </c>
-      <c r="B78" s="12" t="n">
+      <c r="B78" s="2" t="n">
         <v>45867</v>
       </c>
       <c r="C78" t="inlineStr">
@@ -2658,13 +3267,23 @@
       </c>
       <c r="F78" t="n">
         <v>25000000</v>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
         <v>78</v>
       </c>
-      <c r="B79" s="12" t="n">
+      <c r="B79" s="2" t="n">
         <v>45867</v>
       </c>
       <c r="C79" t="inlineStr">
@@ -2684,13 +3303,23 @@
       </c>
       <c r="F79" t="n">
         <v>13750000</v>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
         <v>79</v>
       </c>
-      <c r="B80" s="12" t="n">
+      <c r="B80" s="2" t="n">
         <v>45867</v>
       </c>
       <c r="C80" t="inlineStr">
@@ -2710,13 +3339,23 @@
       </c>
       <c r="F80" t="n">
         <v>36200000</v>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
         <v>80</v>
       </c>
-      <c r="B81" s="12" t="n">
+      <c r="B81" s="2" t="n">
         <v>45868</v>
       </c>
       <c r="C81" t="inlineStr">
@@ -2736,13 +3375,23 @@
       </c>
       <c r="F81" t="n">
         <v>40000000</v>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
         <v>81</v>
       </c>
-      <c r="B82" s="12" t="n">
+      <c r="B82" s="2" t="n">
         <v>45870</v>
       </c>
       <c r="C82" t="inlineStr">
@@ -2762,13 +3411,23 @@
       </c>
       <c r="F82" t="n">
         <v>50000000</v>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
         <v>82</v>
       </c>
-      <c r="B83" s="12" t="n">
+      <c r="B83" s="2" t="n">
         <v>45877</v>
       </c>
       <c r="C83" t="inlineStr">
@@ -2788,13 +3447,23 @@
       </c>
       <c r="F83" t="n">
         <v>0</v>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
         <v>83</v>
       </c>
-      <c r="B84" s="12" t="n">
+      <c r="B84" s="2" t="n">
         <v>45828</v>
       </c>
       <c r="C84" t="inlineStr">
@@ -2814,13 +3483,23 @@
       </c>
       <c r="F84" t="n">
         <v>388594900</v>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
         <v>84</v>
       </c>
-      <c r="B85" s="12" t="n">
+      <c r="B85" s="2" t="n">
         <v>45832</v>
       </c>
       <c r="C85" t="inlineStr">
@@ -2840,13 +3519,23 @@
       </c>
       <c r="F85" t="n">
         <v>100000000</v>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
         <v>85</v>
       </c>
-      <c r="B86" s="12" t="n">
+      <c r="B86" s="2" t="n">
         <v>45834</v>
       </c>
       <c r="C86" t="inlineStr">
@@ -2866,13 +3555,23 @@
       </c>
       <c r="F86" t="n">
         <v>22000000</v>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
         <v>86</v>
       </c>
-      <c r="B87" s="12" t="n">
+      <c r="B87" s="2" t="n">
         <v>45834</v>
       </c>
       <c r="C87" t="inlineStr">
@@ -2892,13 +3591,23 @@
       </c>
       <c r="F87" t="n">
         <v>20000000</v>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
         <v>87</v>
       </c>
-      <c r="B88" s="12" t="n">
+      <c r="B88" s="2" t="n">
         <v>45834</v>
       </c>
       <c r="C88" t="inlineStr">
@@ -2918,13 +3627,23 @@
       </c>
       <c r="F88" t="n">
         <v>4600000</v>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
         <v>88</v>
       </c>
-      <c r="B89" s="12" t="n">
+      <c r="B89" s="2" t="n">
         <v>45835</v>
       </c>
       <c r="C89" t="inlineStr">
@@ -2944,13 +3663,23 @@
       </c>
       <c r="F89" t="n">
         <v>13500000</v>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
         <v>89</v>
       </c>
-      <c r="B90" s="12" t="n">
+      <c r="B90" s="2" t="n">
         <v>45835</v>
       </c>
       <c r="C90" t="inlineStr">
@@ -2970,13 +3699,23 @@
       </c>
       <c r="F90" t="n">
         <v>6500000</v>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
         <v>90</v>
       </c>
-      <c r="B91" s="12" t="n">
+      <c r="B91" s="2" t="n">
         <v>45841</v>
       </c>
       <c r="C91" t="inlineStr">
@@ -2996,13 +3735,23 @@
       </c>
       <c r="F91" t="n">
         <v>22000000</v>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
         <v>91</v>
       </c>
-      <c r="B92" s="12" t="n">
+      <c r="B92" s="2" t="n">
         <v>45841</v>
       </c>
       <c r="C92" t="inlineStr">
@@ -3022,13 +3771,23 @@
       </c>
       <c r="F92" t="n">
         <v>19000000</v>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
         <v>92</v>
       </c>
-      <c r="B93" s="12" t="n">
+      <c r="B93" s="2" t="n">
         <v>45843</v>
       </c>
       <c r="C93" t="inlineStr">
@@ -3048,13 +3807,23 @@
       </c>
       <c r="F93" t="n">
         <v>50000000</v>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
         <v>93</v>
       </c>
-      <c r="B94" s="12" t="n">
+      <c r="B94" s="2" t="n">
         <v>45848</v>
       </c>
       <c r="C94" t="inlineStr">
@@ -3074,13 +3843,23 @@
       </c>
       <c r="F94" t="n">
         <v>37000000</v>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
         <v>94</v>
       </c>
-      <c r="B95" s="12" t="n">
+      <c r="B95" s="2" t="n">
         <v>45848</v>
       </c>
       <c r="C95" t="inlineStr">
@@ -3100,13 +3879,23 @@
       </c>
       <c r="F95" t="n">
         <v>19300000</v>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
         <v>95</v>
       </c>
-      <c r="B96" s="12" t="n">
+      <c r="B96" s="2" t="n">
         <v>45861</v>
       </c>
       <c r="C96" t="inlineStr">
@@ -3126,13 +3915,23 @@
       </c>
       <c r="F96" t="n">
         <v>78000000</v>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
         <v>96</v>
       </c>
-      <c r="B97" s="12" t="n">
+      <c r="B97" s="2" t="n">
         <v>45863</v>
       </c>
       <c r="C97" t="inlineStr">
@@ -3152,13 +3951,23 @@
       </c>
       <c r="F97" t="n">
         <v>42000000</v>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
         <v>97</v>
       </c>
-      <c r="B98" s="12" t="n">
+      <c r="B98" s="2" t="n">
         <v>45815</v>
       </c>
       <c r="C98" t="inlineStr">
@@ -3178,13 +3987,23 @@
       </c>
       <c r="F98" t="n">
         <v>361771600</v>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
         <v>98</v>
       </c>
-      <c r="B99" s="12" t="n">
+      <c r="B99" s="2" t="n">
         <v>45813</v>
       </c>
       <c r="C99" t="inlineStr">
@@ -3204,13 +4023,23 @@
       </c>
       <c r="F99" t="n">
         <v>44950000</v>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
         <v>99</v>
       </c>
-      <c r="B100" s="12" t="n">
+      <c r="B100" s="2" t="n">
         <v>45814</v>
       </c>
       <c r="C100" t="inlineStr">
@@ -3230,13 +4059,23 @@
       </c>
       <c r="F100" t="n">
         <v>20000000</v>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
         <v>100</v>
       </c>
-      <c r="B101" s="12" t="n">
+      <c r="B101" s="2" t="n">
         <v>45814</v>
       </c>
       <c r="C101" t="inlineStr">
@@ -3256,13 +4095,23 @@
       </c>
       <c r="F101" t="n">
         <v>50000000</v>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
         <v>101</v>
       </c>
-      <c r="B102" s="12" t="n">
+      <c r="B102" s="2" t="n">
         <v>45815</v>
       </c>
       <c r="C102" t="inlineStr">
@@ -3282,13 +4131,23 @@
       </c>
       <c r="F102" t="n">
         <v>9900000</v>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
         <v>102</v>
       </c>
-      <c r="B103" s="12" t="n">
+      <c r="B103" s="2" t="n">
         <v>45816</v>
       </c>
       <c r="C103" t="inlineStr">
@@ -3308,13 +4167,23 @@
       </c>
       <c r="F103" t="n">
         <v>12000000</v>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
         <v>103</v>
       </c>
-      <c r="B104" s="12" t="n">
+      <c r="B104" s="2" t="n">
         <v>45816</v>
       </c>
       <c r="C104" t="inlineStr">
@@ -3334,13 +4203,23 @@
       </c>
       <c r="F104" t="n">
         <v>6000000</v>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
         <v>104</v>
       </c>
-      <c r="B105" s="12" t="n">
+      <c r="B105" s="2" t="n">
         <v>45816</v>
       </c>
       <c r="C105" t="inlineStr">
@@ -3360,13 +4239,23 @@
       </c>
       <c r="F105" t="n">
         <v>2000000</v>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
         <v>105</v>
       </c>
-      <c r="B106" s="12" t="n">
+      <c r="B106" s="2" t="n">
         <v>45816</v>
       </c>
       <c r="C106" t="inlineStr">
@@ -3386,13 +4275,23 @@
       </c>
       <c r="F106" t="n">
         <v>100000</v>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
         <v>106</v>
       </c>
-      <c r="B107" s="12" t="n">
+      <c r="B107" s="2" t="n">
         <v>45819</v>
       </c>
       <c r="C107" t="inlineStr">
@@ -3412,13 +4311,23 @@
       </c>
       <c r="F107" t="n">
         <v>50000000</v>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
         <v>107</v>
       </c>
-      <c r="B108" s="12" t="n">
+      <c r="B108" s="2" t="n">
         <v>45821</v>
       </c>
       <c r="C108" t="inlineStr">
@@ -3438,13 +4347,23 @@
       </c>
       <c r="F108" t="n">
         <v>50000000</v>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
         <v>108</v>
       </c>
-      <c r="B109" s="12" t="n">
+      <c r="B109" s="2" t="n">
         <v>45822</v>
       </c>
       <c r="C109" t="inlineStr">
@@ -3464,13 +4383,23 @@
       </c>
       <c r="F109" t="n">
         <v>15000000</v>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
         <v>109</v>
       </c>
-      <c r="B110" s="12" t="n">
+      <c r="B110" s="2" t="n">
         <v>45822</v>
       </c>
       <c r="C110" t="inlineStr">
@@ -3490,13 +4419,23 @@
       </c>
       <c r="F110" t="n">
         <v>10000000</v>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
         <v>110</v>
       </c>
-      <c r="B111" s="12" t="n">
+      <c r="B111" s="2" t="n">
         <v>45826</v>
       </c>
       <c r="C111" t="inlineStr">
@@ -3516,13 +4455,23 @@
       </c>
       <c r="F111" t="n">
         <v>10000000</v>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
         <v>111</v>
       </c>
-      <c r="B112" s="12" t="n">
+      <c r="B112" s="2" t="n">
         <v>45835</v>
       </c>
       <c r="C112" t="inlineStr">
@@ -3542,13 +4491,23 @@
       </c>
       <c r="F112" t="n">
         <v>14140000</v>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
         <v>112</v>
       </c>
-      <c r="B113" s="12" t="n">
+      <c r="B113" s="2" t="n">
         <v>45835</v>
       </c>
       <c r="C113" t="inlineStr">
@@ -3568,13 +4527,23 @@
       </c>
       <c r="F113" t="n">
         <v>25860000</v>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
         <v>113</v>
       </c>
-      <c r="B114" s="12" t="n">
+      <c r="B114" s="2" t="n">
         <v>45848</v>
       </c>
       <c r="C114" t="inlineStr">
@@ -3594,13 +4563,23 @@
       </c>
       <c r="F114" t="n">
         <v>10655000</v>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
         <v>114</v>
       </c>
-      <c r="B115" s="12" t="n">
+      <c r="B115" s="2" t="n">
         <v>45842</v>
       </c>
       <c r="C115" t="inlineStr">
@@ -3620,13 +4599,23 @@
       </c>
       <c r="F115" t="n">
         <v>27150000</v>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
         <v>115</v>
       </c>
-      <c r="B116" s="12" t="n">
+      <c r="B116" s="2" t="n">
         <v>45842</v>
       </c>
       <c r="C116" t="inlineStr">
@@ -3646,13 +4635,23 @@
       </c>
       <c r="F116" t="n">
         <v>2850000</v>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
         <v>116</v>
       </c>
-      <c r="B117" s="12" t="n">
+      <c r="B117" s="2" t="n">
         <v>45842</v>
       </c>
       <c r="C117" t="inlineStr">
@@ -3672,13 +4671,23 @@
       </c>
       <c r="F117" t="n">
         <v>8000000</v>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
         <v>117</v>
       </c>
-      <c r="B118" s="12" t="n">
+      <c r="B118" s="2" t="n">
         <v>45843</v>
       </c>
       <c r="C118" t="inlineStr">
@@ -3698,13 +4707,23 @@
       </c>
       <c r="F118" t="n">
         <v>5950000</v>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
         <v>118</v>
       </c>
-      <c r="B119" s="12" t="n">
+      <c r="B119" s="2" t="n">
         <v>45843</v>
       </c>
       <c r="C119" t="inlineStr">
@@ -3724,13 +4743,23 @@
       </c>
       <c r="F119" t="n">
         <v>55001700</v>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
         <v>119</v>
       </c>
-      <c r="B120" s="12" t="n">
+      <c r="B120" s="2" t="n">
         <v>45846</v>
       </c>
       <c r="C120" t="inlineStr">
@@ -3750,13 +4779,23 @@
       </c>
       <c r="F120" t="n">
         <v>15000000</v>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
         <v>120</v>
       </c>
-      <c r="B121" s="12" t="n">
+      <c r="B121" s="2" t="n">
         <v>45847</v>
       </c>
       <c r="C121" t="inlineStr">
@@ -3776,13 +4815,23 @@
       </c>
       <c r="F121" t="n">
         <v>27087600</v>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
         <v>121</v>
       </c>
-      <c r="B122" s="12" t="n">
+      <c r="B122" s="2" t="n">
         <v>45849</v>
       </c>
       <c r="C122" t="inlineStr">
@@ -3802,13 +4851,23 @@
       </c>
       <c r="F122" t="n">
         <v>25000000</v>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
         <v>122</v>
       </c>
-      <c r="B123" s="12" t="n">
+      <c r="B123" s="2" t="n">
         <v>45849</v>
       </c>
       <c r="C123" t="inlineStr">
@@ -3828,13 +4887,23 @@
       </c>
       <c r="F123" t="n">
         <v>40000000</v>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
         <v>123</v>
       </c>
-      <c r="B124" s="12" t="n">
+      <c r="B124" s="2" t="n">
         <v>45850</v>
       </c>
       <c r="C124" t="inlineStr">
@@ -3854,13 +4923,23 @@
       </c>
       <c r="F124" t="n">
         <v>231669450</v>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
         <v>124</v>
       </c>
-      <c r="B125" s="12" t="n">
+      <c r="B125" s="2" t="n">
         <v>45863</v>
       </c>
       <c r="C125" t="inlineStr">
@@ -3880,13 +4959,23 @@
       </c>
       <c r="F125" t="n">
         <v>20000000</v>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
         <v>125</v>
       </c>
-      <c r="B126" s="12" t="n">
+      <c r="B126" s="2" t="n">
         <v>45867</v>
       </c>
       <c r="C126" t="inlineStr">
@@ -3906,13 +4995,23 @@
       </c>
       <c r="F126" t="n">
         <v>2600000</v>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
         <v>126</v>
       </c>
-      <c r="B127" s="12" t="n">
+      <c r="B127" s="2" t="n">
         <v>45863</v>
       </c>
       <c r="C127" t="inlineStr">
@@ -3932,13 +5031,23 @@
       </c>
       <c r="F127" t="n">
         <v>25000000</v>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
         <v>127</v>
       </c>
-      <c r="B128" s="12" t="n">
+      <c r="B128" s="2" t="n">
         <v>45867</v>
       </c>
       <c r="C128" t="inlineStr">
@@ -3958,13 +5067,23 @@
       </c>
       <c r="F128" t="n">
         <v>400000</v>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
         <v>128</v>
       </c>
-      <c r="B129" s="12" t="n">
+      <c r="B129" s="2" t="n">
         <v>45869</v>
       </c>
       <c r="C129" t="inlineStr">
@@ -3984,13 +5103,23 @@
       </c>
       <c r="F129" t="n">
         <v>25000000</v>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
         <v>129</v>
       </c>
-      <c r="B130" s="12" t="n">
+      <c r="B130" s="2" t="n">
         <v>45870</v>
       </c>
       <c r="C130" t="inlineStr">
@@ -4010,13 +5139,23 @@
       </c>
       <c r="F130" t="n">
         <v>17922000</v>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
         <v>130</v>
       </c>
-      <c r="B131" s="12" t="n">
+      <c r="B131" s="2" t="n">
         <v>45875</v>
       </c>
       <c r="C131" t="inlineStr">
@@ -4036,13 +5175,23 @@
       </c>
       <c r="F131" t="n">
         <v>22600000</v>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
         <v>131</v>
       </c>
-      <c r="B132" s="12" t="n">
+      <c r="B132" s="2" t="n">
         <v>45869</v>
       </c>
       <c r="C132" t="inlineStr">
@@ -4062,13 +5211,23 @@
       </c>
       <c r="F132" t="n">
         <v>101681900</v>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
         <v>132</v>
       </c>
-      <c r="B133" s="12" t="n">
+      <c r="B133" s="2" t="n">
         <v>45869</v>
       </c>
       <c r="C133" t="inlineStr">
@@ -4088,13 +5247,23 @@
       </c>
       <c r="F133" t="n">
         <v>15000000</v>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
         <v>133</v>
       </c>
-      <c r="B134" s="12" t="n">
+      <c r="B134" s="2" t="n">
         <v>45869</v>
       </c>
       <c r="C134" t="inlineStr">
@@ -4114,13 +5283,23 @@
       </c>
       <c r="F134" t="n">
         <v>5000000</v>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
         <v>134</v>
       </c>
-      <c r="B135" s="12" t="n">
+      <c r="B135" s="2" t="n">
         <v>45869</v>
       </c>
       <c r="C135" t="inlineStr">
@@ -4140,13 +5319,23 @@
       </c>
       <c r="F135" t="n">
         <v>40000000</v>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
         <v>135</v>
       </c>
-      <c r="B136" s="12" t="n">
+      <c r="B136" s="2" t="n">
         <v>45869</v>
       </c>
       <c r="C136" t="inlineStr">
@@ -4166,13 +5355,23 @@
       </c>
       <c r="F136" t="n">
         <v>23000000</v>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
         <v>136</v>
       </c>
-      <c r="B137" s="12" t="n">
+      <c r="B137" s="2" t="n">
         <v>45870</v>
       </c>
       <c r="C137" t="inlineStr">
@@ -4192,13 +5391,23 @@
       </c>
       <c r="F137" t="n">
         <v>1000000</v>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
         <v>137</v>
       </c>
-      <c r="B138" s="12" t="n">
+      <c r="B138" s="2" t="n">
         <v>45870</v>
       </c>
       <c r="C138" t="inlineStr">
@@ -4218,13 +5427,23 @@
       </c>
       <c r="F138" t="n">
         <v>56521700</v>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
         <v>138</v>
       </c>
-      <c r="B139" s="12" t="n">
+      <c r="B139" s="2" t="n">
         <v>45872</v>
       </c>
       <c r="C139" t="inlineStr">
@@ -4244,13 +5463,23 @@
       </c>
       <c r="F139" t="n">
         <v>46153800</v>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
         <v>139</v>
       </c>
-      <c r="B140" s="12" t="n">
+      <c r="B140" s="2" t="n">
         <v>45873</v>
       </c>
       <c r="C140" t="inlineStr">
@@ -4270,13 +5499,23 @@
       </c>
       <c r="F140" t="n">
         <v>15386000</v>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
         <v>140</v>
       </c>
-      <c r="B141" s="12" t="n">
+      <c r="B141" s="2" t="n">
         <v>45873</v>
       </c>
       <c r="C141" t="inlineStr">
@@ -4296,13 +5535,23 @@
       </c>
       <c r="F141" t="n">
         <v>2000000</v>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
         <v>141</v>
       </c>
-      <c r="B142" s="12" t="n">
+      <c r="B142" s="2" t="n">
         <v>45877</v>
       </c>
       <c r="C142" t="inlineStr">
@@ -4322,13 +5571,23 @@
       </c>
       <c r="F142" t="n">
         <v>38000000</v>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
         <v>142</v>
       </c>
-      <c r="B143" s="12" t="n">
+      <c r="B143" s="2" t="n">
         <v>45875</v>
       </c>
       <c r="C143" t="inlineStr">
@@ -4348,13 +5607,23 @@
       </c>
       <c r="F143" t="n">
         <v>22000000</v>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
         <v>143</v>
       </c>
-      <c r="B144" s="12" t="n">
+      <c r="B144" s="2" t="n">
         <v>45875</v>
       </c>
       <c r="C144" t="inlineStr">
@@ -4374,13 +5643,23 @@
       </c>
       <c r="F144" t="n">
         <v>22000000</v>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
         <v>144</v>
       </c>
-      <c r="B145" s="12" t="n">
+      <c r="B145" s="2" t="n">
         <v>45875</v>
       </c>
       <c r="C145" t="inlineStr">
@@ -4400,13 +5679,23 @@
       </c>
       <c r="F145" t="n">
         <v>20000000</v>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
         <v>145</v>
       </c>
-      <c r="B146" s="12" t="n">
+      <c r="B146" s="2" t="n">
         <v>45875</v>
       </c>
       <c r="C146" t="inlineStr">
@@ -4426,13 +5715,23 @@
       </c>
       <c r="F146" t="n">
         <v>36640500</v>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
         <v>146</v>
       </c>
-      <c r="B147" s="12" t="n">
+      <c r="B147" s="2" t="n">
         <v>45877</v>
       </c>
       <c r="C147" t="inlineStr">
@@ -4452,13 +5751,23 @@
       </c>
       <c r="F147" t="n">
         <v>20000000</v>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
         <v>147</v>
       </c>
-      <c r="B148" s="12" t="n">
+      <c r="B148" s="2" t="n">
         <v>45860</v>
       </c>
       <c r="C148" t="inlineStr">
@@ -4479,57 +5788,382 @@
       <c r="F148" t="n">
         <v>57654400</v>
       </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>148</v>
+      </c>
+      <c r="B149" s="2" t="n">
+        <v>45909</v>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="F149" t="n">
+        <v>50000</v>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>Inactiva</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>149</v>
+      </c>
+      <c r="B150" s="2" t="n">
+        <v>45909</v>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F150" t="n">
+        <v>50000</v>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>Inactiva</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>150</v>
+      </c>
+      <c r="B151" s="2" t="n">
+        <v>45909</v>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="F151" t="n">
+        <v>50000</v>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>F-002</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>151</v>
+      </c>
+      <c r="B152" s="2" t="n">
+        <v>45909</v>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F152" t="n">
+        <v>45000</v>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>F-002</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>152</v>
+      </c>
+      <c r="B153" s="2" t="n">
+        <v>45901</v>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F153" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>F-002</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>153</v>
+      </c>
+      <c r="B154" s="2" t="n">
+        <v>45903</v>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F154" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>F-002</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>154</v>
+      </c>
+      <c r="B155" s="3" t="n">
+        <v>45910</v>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F155" t="n">
+        <v>100</v>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>F-002</t>
+        </is>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>155</v>
+      </c>
+      <c r="B156" s="2" t="n">
+        <v>45910</v>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F156" t="n">
+        <v>0</v>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>F-002</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>156</v>
+      </c>
+      <c r="B157" s="2" t="n">
+        <v>45910</v>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F157" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>F-002</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Hoja2">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="A1" sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="21" customWidth="1" min="2" max="2"/>
-    <col width="17.109375" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="15.33203125" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="15" bestFit="1" customWidth="1" min="5" max="5"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="8" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Id</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Proveedor</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Total Facturas</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Total Abonos</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Saldo</t>
         </is>
@@ -4649,11 +6283,27 @@
         <v>64971400</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>49100</v>
+      </c>
+      <c r="E8" t="n">
+        <v>900</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -4663,43 +6313,56 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="32.33203125" customWidth="1" style="1" min="2" max="2"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Id</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Fecha </t>
-        </is>
-      </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
         <is>
           <t>Proveedor</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Detalle</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
-        <is>
-          <t>Observación</t>
-        </is>
-      </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Obs</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
         <is>
           <t>Total</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>IdFactura</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Estado</t>
         </is>
       </c>
     </row>
@@ -4707,12 +6370,12 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="n">
+      <c r="B2" s="1" t="n">
         <v>45880</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Pepito</t>
+          <t>Abimelec</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -4728,10 +6391,199 @@
       <c r="F2" t="n">
         <v>50000000</v>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Inactiva</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>45909</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Abimelec</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>50000000</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>F-001</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Inactiva</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>45909</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Abimelec</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>50000</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>F-002</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Inactiva</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>45909</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Abimelec</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Total Factura : 50000 + saldo anterior 50000 = total 100000</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>100000</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>F-003</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>45909</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Abimelec</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>70000</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>F-003</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>45909</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Abimelec</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Abono</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>F-003</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -4743,34 +6595,34 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" ht="28.8" customHeight="1">
-      <c r="A1" s="8" t="inlineStr">
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Id</t>
         </is>
       </c>
-      <c r="B1" s="8" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Proveedor</t>
         </is>
       </c>
-      <c r="C1" s="9" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Total Facturas</t>
         </is>
       </c>
-      <c r="D1" s="9" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Total Abonos</t>
         </is>
       </c>
-      <c r="E1" s="10" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Saldo</t>
         </is>
@@ -4782,17 +6634,149 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Pepito</t>
+          <t>Abimelec</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>50000000</v>
+        <v>100000</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>72000</v>
       </c>
       <c r="E2" t="n">
-        <v>50000000</v>
+        <v>28000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="16.88671875" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Categoria</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Placa</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Conductor</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Precio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>45908</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Flete</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ZIW41G</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>45901</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Parqueadero</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>YRF47E</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Abimelec</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>45906</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Varios</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>YRF47E</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Abimelec</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>50000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>